<commit_message>
This is fifth commit
</commit_message>
<xml_diff>
--- a/OOPs/HYE Marks.xlsx
+++ b/OOPs/HYE Marks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\AP\Alok_Civil_BMSCE\OOPs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46F7EB38-1ACE-4AC9-8E08-338B5E1551C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4DF2779-463C-40F3-AC7A-895A2B37B0B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="143">
   <si>
     <t>S.No.</t>
   </si>
@@ -403,21 +403,6 @@
     <t>Tiqida</t>
   </si>
   <si>
-    <t>Test1</t>
-  </si>
-  <si>
-    <t>Test2</t>
-  </si>
-  <si>
-    <t>Test3</t>
-  </si>
-  <si>
-    <t>Test4</t>
-  </si>
-  <si>
-    <t>Test5</t>
-  </si>
-  <si>
     <t>CO1</t>
   </si>
   <si>
@@ -461,6 +446,24 @@
   </si>
   <si>
     <t>CO4</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>Q4</t>
+  </si>
+  <si>
+    <t>Q5</t>
+  </si>
+  <si>
+    <t>maxMarks</t>
   </si>
 </sst>
 </file>
@@ -482,12 +485,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -502,7 +523,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -514,6 +535,14 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -799,76 +828,80 @@
   <dimension ref="A1:H62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="8" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>126</v>
+      <c r="D1" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C2" t="s">
+      <c r="C2" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="8">
         <v>1</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="8">
+        <v>1</v>
+      </c>
+      <c r="F2" s="8">
         <v>2</v>
       </c>
-      <c r="F2" s="1">
-        <v>2</v>
-      </c>
-      <c r="G2" s="1">
+      <c r="G2" s="8">
         <v>3</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="8">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D3" s="1">
+      <c r="C3" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="D3" s="8">
         <v>20</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="8">
         <v>20</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="8">
         <v>20</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="8">
         <v>20</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="8">
         <v>20</v>
       </c>
     </row>
@@ -2418,7 +2451,7 @@
   <dimension ref="A1:O63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2438,42 +2471,42 @@
     <row r="2" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="3" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D3" s="1">
         <v>3</v>
@@ -2511,7 +2544,7 @@
     </row>
     <row r="4" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D4" s="1">
         <v>3</v>
@@ -2549,7 +2582,7 @@
     </row>
     <row r="5" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D5" s="1">
         <v>2</v>
@@ -2587,16 +2620,16 @@
     </row>
     <row r="6" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D6" s="1">
         <v>0</v>
       </c>
       <c r="E6" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F6" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G6" s="1">
         <v>0</v>
@@ -2605,7 +2638,7 @@
         <v>0</v>
       </c>
       <c r="I6" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J6" s="1">
         <v>0</v>
@@ -2646,7 +2679,7 @@
     </row>
     <row r="10" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -2654,12 +2687,12 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="O10" s="1" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -2667,12 +2700,12 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="O11" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -2680,12 +2713,12 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="O12" s="1" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -2693,7 +2726,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="O13" s="1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="14" spans="3:15" x14ac:dyDescent="0.25">
@@ -2703,7 +2736,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="O14" s="1" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="15" spans="3:15" x14ac:dyDescent="0.25">
@@ -2713,7 +2746,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="O15" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="16" spans="3:15" x14ac:dyDescent="0.25">
@@ -2723,7 +2756,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="O16" s="1" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" spans="4:15" x14ac:dyDescent="0.25">
@@ -2733,7 +2766,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="O17" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" spans="4:15" x14ac:dyDescent="0.25">
@@ -2743,7 +2776,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="O18" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="4:15" x14ac:dyDescent="0.25">
@@ -2753,7 +2786,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="O19" s="1" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="20" spans="4:15" x14ac:dyDescent="0.25">
@@ -2763,7 +2796,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="O20" s="1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="21" spans="4:15" x14ac:dyDescent="0.25">

</xml_diff>